<commit_message>
adding the bestyears to db functionality (not tested)
</commit_message>
<xml_diff>
--- a/Dataset/Output/catalog.xlsx
+++ b/Dataset/Output/catalog.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\School Projects\Sumerian-Social-Network-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\SchoolProjects\Sumerian-Social-Network-Project\Dataset\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E5796C-752E-4952-81DE-C6E4D1E5C0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD0BB3A-A7B9-47AD-A061-A162F5F286D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="11210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yearNames" sheetId="1" r:id="rId1"/>
     <sheet name="placeNames" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1933,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1943,7 +1955,7 @@
     <col min="2" max="2" width="67.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1956,8 +1968,12 @@
       <c r="D1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1">
+        <f>COUNT(D1:D174)</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -1971,7 +1987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1985,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -1999,7 +2015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2013,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -2027,7 +2043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2041,7 +2057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -2055,7 +2071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -2083,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2097,7 +2113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2111,7 +2127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2125,7 +2141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2139,7 +2155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -2153,7 +2169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>

</xml_diff>